<commit_message>
re re re updated since pycharm likes to delete my work
</commit_message>
<xml_diff>
--- a/analysis/data_commit/rob_analysis/others.xlsx
+++ b/analysis/data_commit/rob_analysis/others.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/dev/marks/2024/cpvt_database_analysis/analysis/data_commit/rob_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0537E02E-BC84-DE4D-9730-2D52FED81B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4AEE3C-054C-C243-B7EE-43BCECDC9B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -245,9 +245,6 @@
     <t>https://doi.org/10.3390/jcm7110423</t>
   </si>
   <si>
-    <t>Diagnostic</t>
-  </si>
-  <si>
     <t>Investigating the genetic causes of sudden unexpected death in children through targeted next-generation sequencing analysis</t>
   </si>
   <si>
@@ -288,6 +285,9 @@
   </si>
   <si>
     <t>https://doi.org/10.1016/j.amjcard.2014.09.037</t>
+  </si>
+  <si>
+    <t>Dewar, LJ</t>
   </si>
 </sst>
 </file>
@@ -354,19 +354,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{E58389EC-A806-974F-A1DD-5F6E69D7B85A}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -701,7 +704,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1095,17 +1098,17 @@
       <c r="B14" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="G14" t="b">
         <v>0</v>
@@ -1122,19 +1125,19 @@
         <v>1255</v>
       </c>
       <c r="B15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" t="s">
         <v>73</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>74</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>75</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>76</v>
-      </c>
-      <c r="F15" t="s">
-        <v>77</v>
       </c>
       <c r="G15" t="b">
         <v>0</v>
@@ -1151,19 +1154,19 @@
         <v>1295</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="G16" t="b">
         <v>0</v>
@@ -1176,11 +1179,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G1" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G21">
-      <sortCondition ref="A1"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update with practical effect size
</commit_message>
<xml_diff>
--- a/analysis/data_commit/rob_analysis/others.xlsx
+++ b/analysis/data_commit/rob_analysis/others.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10119"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cumccolumbia-my.sharepoint.com/personal/ac4294_cumc_columbia_edu/Documents/documents/papers/ryr_database/AHA_circulation-r1/risk of bias/rob_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="155" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36232475-9FC6-704F-ACF3-5822E44FE43E}"/>
+  <xr:revisionPtr revIDLastSave="169" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D523306-DDA2-BA4E-9350-5047F38282F6}"/>
   <bookViews>
-    <workbookView xWindow="24060" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="92">
   <si>
     <t>publication_id</t>
   </si>
@@ -245,12 +245,69 @@
     <t>https://doi.org/10.3390/jcm7110423</t>
   </si>
   <si>
-    <t>Diagnostic</t>
+    <t>Arrhythmogenesis in a catecholaminergic polymorphic ventricular tachycardia mutation that depresses ryanodine receptor function.</t>
+  </si>
+  <si>
+    <t>Zhao YT</t>
+  </si>
+  <si>
+    <t>10.1073/pnas.1419795112</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/25775566</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1073/pnas.1419795112</t>
+  </si>
+  <si>
+    <t>Sudden cardiac death and cardiovascular pathology: from anatomic theater to double helix</t>
+  </si>
+  <si>
+    <t>Thiene, G.</t>
+  </si>
+  <si>
+    <t>10.1016/j.amjcard.2014.09.037</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/25438923</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.amjcard.2014.09.037</t>
+  </si>
+  <si>
+    <t>Genetic Background of Catecholaminergic Polymorphic Ventricular Tachycardia in Japan</t>
+  </si>
+  <si>
+    <t>Kawamura, M</t>
+  </si>
+  <si>
+    <t>10.1253/circj.cj-12-1460</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/23595086</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1253/circj.cj-12-1460</t>
+  </si>
+  <si>
+    <t>Sudden arrhythmia death syndrome in young victims: a five-year retrospective review and two-year prospective molecular autopsy study by next-generation sequencing and clinical evaluation of their first-degree relatives</t>
+  </si>
+  <si>
+    <t>Mak, CM</t>
+  </si>
+  <si>
+    <t>10.12809/hkmj187256</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/30670673</t>
   </si>
   <si>
     <t>Investigating the genetic causes of sudden unexpected death in children through targeted next-generation sequencing analysis</t>
   </si>
   <si>
+    <t>Dewar, L.</t>
+  </si>
+  <si>
     <t>10.1161/CIRCGENETICS.116.001738</t>
   </si>
   <si>
@@ -258,75 +315,6 @@
   </si>
   <si>
     <t>https://doi.org/10.1161/CIRCGENETICS.116.001738</t>
-  </si>
-  <si>
-    <t>Arrhythmogenesis in a catecholaminergic polymorphic ventricular tachycardia mutation that depresses ryanodine receptor function.</t>
-  </si>
-  <si>
-    <t>Zhao YT</t>
-  </si>
-  <si>
-    <t>10.1073/pnas.1419795112</t>
-  </si>
-  <si>
-    <t>https://pubmed.ncbi.nlm.nih.gov/25775566</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1073/pnas.1419795112</t>
-  </si>
-  <si>
-    <t>Sudden cardiac death and cardiovascular pathology: from anatomic theater to double helix</t>
-  </si>
-  <si>
-    <t>Thiene, G.</t>
-  </si>
-  <si>
-    <t>10.1016/j.amjcard.2014.09.037</t>
-  </si>
-  <si>
-    <t>https://pubmed.ncbi.nlm.nih.gov/25438923</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1016/j.amjcard.2014.09.037</t>
-  </si>
-  <si>
-    <t>Genetic Background of Catecholaminergic Polymorphic Ventricular Tachycardia in Japan</t>
-  </si>
-  <si>
-    <t>Kawamura, M</t>
-  </si>
-  <si>
-    <t>10.1253/circj.cj-12-1460</t>
-  </si>
-  <si>
-    <t>https://pubmed.ncbi.nlm.nih.gov/23595086</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1253/circj.cj-12-1460</t>
-  </si>
-  <si>
-    <t>Sudden arrhythmia death syndrome in young victims: a five-year retrospective review and two-year prospective molecular autopsy study by next-generation sequencing and clinical evaluation of their first-degree relatives</t>
-  </si>
-  <si>
-    <t>Mak, CM</t>
-  </si>
-  <si>
-    <t>10.12809/hkmj187256</t>
-  </si>
-  <si>
-    <t>https://pubmed.ncbi.nlm.nih.gov/30670673</t>
-  </si>
-  <si>
-    <t>Prevalence and significance of rare RYR2 variants in arrhythmogenic right ventricular cardiomyopathy/dysplasia: Results of a systematic screening</t>
-  </si>
-  <si>
-    <t>Roux-Buisson, N</t>
-  </si>
-  <si>
-    <t>10.1016/j.hrthm.2014.07.020</t>
-  </si>
-  <si>
-    <t>https://pubmed.ncbi.nlm.nih.gov/25041964</t>
   </si>
 </sst>
 </file>
@@ -361,7 +349,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -371,12 +359,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -408,17 +390,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -757,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+      <selection activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -770,7 +749,7 @@
     <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="224" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -937,7 +916,7 @@
       <c r="G6" t="b">
         <v>0</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6">
         <v>10</v>
       </c>
       <c r="I6">
@@ -1148,95 +1127,95 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
-        <v>1225</v>
-      </c>
-      <c r="B14" s="3" t="s">
+      <c r="A14">
+        <v>1255</v>
+      </c>
+      <c r="B14" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" t="s">
         <v>69</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" t="s">
         <v>71</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" t="s">
         <v>72</v>
       </c>
       <c r="G14" t="b">
         <v>0</v>
       </c>
-      <c r="H14" s="4">
-        <v>10</v>
+      <c r="H14">
+        <v>6</v>
       </c>
       <c r="I14">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>1255</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="A15" s="2">
+        <v>1295</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="2" t="s">
         <v>77</v>
       </c>
       <c r="G15" t="b">
         <v>0</v>
       </c>
       <c r="H15">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>4</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" s="3">
+        <v>10</v>
+      </c>
+      <c r="I16" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
-        <v>1295</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G16" t="b">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>7</v>
-      </c>
-      <c r="I16">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
-        <v>4</v>
+        <v>1193</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>83</v>
@@ -1250,76 +1229,47 @@
       <c r="E17" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="3" t="str">
+        <f t="shared" ref="F17" si="0">IF(D17&lt;&gt;"N/A",_xlfn.CONCAT("https://doi.org/",D17),"")</f>
+        <v>https://doi.org/10.12809/hkmj187256</v>
+      </c>
+      <c r="G17" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" s="3">
+        <v>11</v>
+      </c>
+      <c r="I17" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>1225</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="G17" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H17" s="4">
+      <c r="C18" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" s="3" t="b">
+        <f>IF(I18=1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="3">
         <v>10</v>
       </c>
-      <c r="I17" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="5">
-        <v>1193</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="F18" s="4" t="str">
-        <f t="shared" ref="F18" si="0">IF(D18&lt;&gt;"N/A",_xlfn.CONCAT("https://doi.org/",D18),"")</f>
-        <v>https://doi.org/10.12809/hkmj187256</v>
-      </c>
-      <c r="G18" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>11</v>
-      </c>
-      <c r="I18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="6">
-        <v>16</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F19" s="7" t="str">
-        <f t="shared" ref="F19" si="1">IF(D19&lt;&gt;"N/A",_xlfn.CONCAT("https://doi.org/",D19),"")</f>
-        <v>https://doi.org/10.1016/j.hrthm.2014.07.020</v>
-      </c>
-      <c r="G19" t="b">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>10</v>
-      </c>
-      <c r="I19">
+      <c r="I18" s="3">
         <v>5</v>
       </c>
     </row>

</xml_diff>